<commit_message>
Asignacion de trabajo para la iteracion 4
</commit_message>
<xml_diff>
--- a/docs/2.0/Control.xlsx
+++ b/docs/2.0/Control.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="131">
   <si>
     <t>Caso de uso</t>
   </si>
@@ -303,9 +303,6 @@
     <t>View/maquinas/listarExterno.php</t>
   </si>
   <si>
-    <t>1.3,3.2</t>
-  </si>
-  <si>
     <t>View/incidencias/listarExterno.php</t>
   </si>
   <si>
@@ -393,16 +390,43 @@
     <t>Marco Y Héctor: revisión general y puesta a punto del sistema online</t>
   </si>
   <si>
-    <t>Alejandro: investigar multi-idioma</t>
-  </si>
-  <si>
-    <t>Diego: prueba de funcionalidades</t>
+    <t>No(Abado por otro recurso)</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>1.4,1.5</t>
+  </si>
+  <si>
+    <t>1.2,1.6</t>
+  </si>
+  <si>
+    <t>2.2,2.4,2.6</t>
+  </si>
+  <si>
+    <t>3.1,3.2,3.3</t>
+  </si>
+  <si>
+    <t>3.4,3.5,3.6,3.7</t>
+  </si>
+  <si>
+    <t>3.9,3.10</t>
+  </si>
+  <si>
+    <t>Alejandro: Multi-idiomas</t>
+  </si>
+  <si>
+    <t>Iteracion 4 - Fecha límite de entrega: 9 de septiembre antes de las 17:00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00_);\(0.00\)"/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -804,7 +828,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -889,6 +913,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1223,10 +1250,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ48"/>
+  <dimension ref="A1:AQ48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W3" workbookViewId="0">
-      <selection activeCell="AG26" sqref="AG26"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AL2" sqref="AL2:AQ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1240,130 +1267,161 @@
     <col min="8" max="8" width="10" customWidth="1"/>
     <col min="9" max="9" width="41" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="41.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.7109375" customWidth="1"/>
-    <col min="18" max="18" width="10.7109375" style="20" customWidth="1"/>
-    <col min="19" max="19" width="15.7109375" customWidth="1"/>
-    <col min="20" max="20" width="10.7109375" style="20" customWidth="1"/>
-    <col min="21" max="21" width="15.7109375" customWidth="1"/>
-    <col min="22" max="22" width="10.7109375" style="20" customWidth="1"/>
-    <col min="24" max="24" width="15.7109375" customWidth="1"/>
-    <col min="26" max="26" width="15.7109375" customWidth="1"/>
-    <col min="28" max="28" width="15.7109375" customWidth="1"/>
+    <col min="15" max="15" width="13" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.5703125" customWidth="1"/>
+    <col min="17" max="17" width="3" customWidth="1"/>
+    <col min="18" max="18" width="4.28515625" style="20" customWidth="1"/>
+    <col min="19" max="19" width="3.28515625" customWidth="1"/>
+    <col min="20" max="20" width="1.5703125" style="20" customWidth="1"/>
+    <col min="21" max="21" width="2.140625" customWidth="1"/>
+    <col min="22" max="22" width="2.28515625" style="20" customWidth="1"/>
+    <col min="23" max="23" width="2.140625" customWidth="1"/>
+    <col min="24" max="24" width="2.5703125" customWidth="1"/>
+    <col min="25" max="25" width="2.7109375" customWidth="1"/>
+    <col min="26" max="26" width="4.28515625" customWidth="1"/>
+    <col min="27" max="27" width="4" customWidth="1"/>
+    <col min="28" max="28" width="3.5703125" customWidth="1"/>
+    <col min="29" max="29" width="4.28515625" customWidth="1"/>
+    <col min="30" max="30" width="2.7109375" customWidth="1"/>
+    <col min="31" max="31" width="3.85546875" customWidth="1"/>
+    <col min="32" max="33" width="5.5703125" customWidth="1"/>
+    <col min="34" max="34" width="5.42578125" customWidth="1"/>
+    <col min="35" max="35" width="2.42578125" customWidth="1"/>
+    <col min="36" max="36" width="3.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="43" t="s">
+    <row r="1" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="43"/>
+      <c r="B2" s="44"/>
       <c r="C2" s="8" t="s">
         <v>24</v>
       </c>
       <c r="D2" s="8"/>
-      <c r="E2" s="43" t="s">
+      <c r="E2" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
-      <c r="N2" s="43"/>
-      <c r="O2" s="43"/>
-      <c r="Q2" s="38" t="s">
-        <v>102</v>
-      </c>
-      <c r="R2" s="39"/>
-      <c r="S2" s="39"/>
-      <c r="T2" s="39"/>
-      <c r="U2" s="39"/>
-      <c r="V2" s="40"/>
-      <c r="X2" s="38" t="s">
-        <v>112</v>
-      </c>
-      <c r="Y2" s="39"/>
-      <c r="Z2" s="39"/>
-      <c r="AA2" s="39"/>
-      <c r="AB2" s="39"/>
-      <c r="AC2" s="40"/>
-      <c r="AE2" s="38" t="s">
-        <v>120</v>
-      </c>
-      <c r="AF2" s="39"/>
-      <c r="AG2" s="39"/>
-      <c r="AH2" s="39"/>
-      <c r="AI2" s="39"/>
-      <c r="AJ2" s="40"/>
-    </row>
-    <row r="3" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="48"/>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="49" t="s">
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
+      <c r="Q2" s="39" t="s">
+        <v>101</v>
+      </c>
+      <c r="R2" s="40"/>
+      <c r="S2" s="40"/>
+      <c r="T2" s="40"/>
+      <c r="U2" s="40"/>
+      <c r="V2" s="41"/>
+      <c r="X2" s="39" t="s">
+        <v>111</v>
+      </c>
+      <c r="Y2" s="40"/>
+      <c r="Z2" s="40"/>
+      <c r="AA2" s="40"/>
+      <c r="AB2" s="40"/>
+      <c r="AC2" s="41"/>
+      <c r="AE2" s="39" t="s">
+        <v>119</v>
+      </c>
+      <c r="AF2" s="40"/>
+      <c r="AG2" s="40"/>
+      <c r="AH2" s="40"/>
+      <c r="AI2" s="40"/>
+      <c r="AJ2" s="41"/>
+      <c r="AL2" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="AM2" s="40"/>
+      <c r="AN2" s="40"/>
+      <c r="AO2" s="40"/>
+      <c r="AP2" s="40"/>
+      <c r="AQ2" s="41"/>
+    </row>
+    <row r="3" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="49"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="52" t="s">
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="44" t="s">
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="45"/>
-      <c r="N3" s="45"/>
-      <c r="O3" s="46"/>
+      <c r="M3" s="46"/>
+      <c r="N3" s="46"/>
+      <c r="O3" s="47"/>
       <c r="P3" s="4"/>
-      <c r="Q3" s="41" t="s">
+      <c r="Q3" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="R3" s="42"/>
-      <c r="S3" s="41" t="s">
-        <v>104</v>
-      </c>
-      <c r="T3" s="42"/>
-      <c r="U3" s="41" t="s">
+      <c r="R3" s="43"/>
+      <c r="S3" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="T3" s="43"/>
+      <c r="U3" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="V3" s="42"/>
-      <c r="X3" s="41" t="s">
+      <c r="V3" s="43"/>
+      <c r="X3" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="Y3" s="42"/>
-      <c r="Z3" s="41" t="s">
-        <v>104</v>
-      </c>
-      <c r="AA3" s="42"/>
-      <c r="AB3" s="41" t="s">
+      <c r="Y3" s="43"/>
+      <c r="Z3" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="AA3" s="43"/>
+      <c r="AB3" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="AC3" s="42"/>
-      <c r="AE3" s="41" t="s">
+      <c r="AC3" s="43"/>
+      <c r="AE3" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="AF3" s="42"/>
-      <c r="AG3" s="41" t="s">
-        <v>104</v>
-      </c>
-      <c r="AH3" s="42"/>
-      <c r="AI3" s="41" t="s">
+      <c r="AF3" s="43"/>
+      <c r="AG3" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="AH3" s="43"/>
+      <c r="AI3" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="AJ3" s="42"/>
-    </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A4" s="48"/>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48"/>
+      <c r="AJ3" s="43"/>
+      <c r="AL3" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM3" s="43"/>
+      <c r="AN3" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="AO3" s="43"/>
+      <c r="AP3" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="AQ3" s="43"/>
+    </row>
+    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A4" s="49"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
       <c r="D4" s="14" t="s">
         <v>64</v>
       </c>
@@ -1402,65 +1460,83 @@
       </c>
       <c r="P4" s="4"/>
       <c r="Q4" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="R4" s="23" t="s">
         <v>52</v>
       </c>
       <c r="S4" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="T4" s="23" t="s">
         <v>52</v>
       </c>
       <c r="U4" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="V4" s="23" t="s">
         <v>52</v>
       </c>
       <c r="X4" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="Y4" s="23" t="s">
         <v>52</v>
       </c>
       <c r="Z4" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AA4" s="23" t="s">
         <v>52</v>
       </c>
       <c r="AB4" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AC4" s="23" t="s">
         <v>52</v>
       </c>
       <c r="AE4" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AF4" s="23" t="s">
         <v>52</v>
       </c>
       <c r="AG4" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AH4" s="23" t="s">
         <v>52</v>
       </c>
       <c r="AI4" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AJ4" s="23" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A5" s="47" t="s">
+      <c r="AL4" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="AM4" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="AN4" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="AO4" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="AP4" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="AQ4" s="23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A5" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="47"/>
+      <c r="B5" s="48"/>
       <c r="C5" s="2"/>
       <c r="D5" s="1" t="s">
         <v>46</v>
@@ -1494,18 +1570,18 @@
       <c r="O5" s="3"/>
       <c r="P5" s="4"/>
       <c r="Q5" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R5" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="S5" s="21"/>
       <c r="T5" s="23"/>
       <c r="U5" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="V5" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="X5" s="21"/>
       <c r="Y5" s="23"/>
@@ -1519,12 +1595,18 @@
       <c r="AH5" s="23"/>
       <c r="AI5" s="21"/>
       <c r="AJ5" s="23"/>
-    </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A6" s="47" t="s">
+      <c r="AL5" s="21"/>
+      <c r="AM5" s="23"/>
+      <c r="AN5" s="21"/>
+      <c r="AO5" s="23"/>
+      <c r="AP5" s="21"/>
+      <c r="AQ5" s="23"/>
+    </row>
+    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A6" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="47"/>
+      <c r="B6" s="48"/>
       <c r="C6" s="2"/>
       <c r="D6" s="1" t="s">
         <v>46</v>
@@ -1532,10 +1614,10 @@
       <c r="E6" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G6" s="3"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="3">
+        <v>1.1000000000000001</v>
+      </c>
       <c r="H6" s="1" t="s">
         <v>46</v>
       </c>
@@ -1553,64 +1635,72 @@
         <v>89</v>
       </c>
       <c r="N6" s="2"/>
-      <c r="O6" s="3">
-        <v>3.1</v>
+      <c r="O6" s="3" t="s">
+        <v>126</v>
       </c>
       <c r="P6" s="4"/>
       <c r="Q6" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="R6" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="S6" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="T6" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="U6" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="R6" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="S6" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="T6" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="U6" s="21" t="s">
-        <v>111</v>
-      </c>
       <c r="V6" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X6" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Y6" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Z6" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA6" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="AB6" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="AA6" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="AB6" s="21" t="s">
-        <v>114</v>
-      </c>
       <c r="AC6" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AE6" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AF6" s="23" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="AG6" s="21"/>
       <c r="AH6" s="23"/>
       <c r="AI6" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="AJ6" s="23"/>
-    </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A7" s="47" t="s">
+        <v>113</v>
+      </c>
+      <c r="AJ6" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="AL6" s="21"/>
+      <c r="AM6" s="23"/>
+      <c r="AN6" s="21"/>
+      <c r="AO6" s="23"/>
+      <c r="AP6" s="21"/>
+      <c r="AQ6" s="23"/>
+    </row>
+    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A7" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="47"/>
+      <c r="B7" s="48"/>
       <c r="C7" s="2"/>
       <c r="D7" s="1" t="s">
         <v>46</v>
@@ -1636,10 +1726,10 @@
       <c r="O7" s="3"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R7" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="S7" s="21"/>
       <c r="T7" s="23"/>
@@ -1657,12 +1747,18 @@
       <c r="AH7" s="23"/>
       <c r="AI7" s="21"/>
       <c r="AJ7" s="23"/>
-    </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A8" s="47" t="s">
+      <c r="AL7" s="21"/>
+      <c r="AM7" s="23"/>
+      <c r="AN7" s="21"/>
+      <c r="AO7" s="23"/>
+      <c r="AP7" s="21"/>
+      <c r="AQ7" s="23"/>
+    </row>
+    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A8" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="47"/>
+      <c r="B8" s="48"/>
       <c r="C8" s="2"/>
       <c r="D8" s="1" t="s">
         <v>46</v>
@@ -1688,20 +1784,20 @@
       <c r="O8" s="3"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R8" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="S8" s="21"/>
       <c r="T8" s="23"/>
       <c r="U8" s="21"/>
       <c r="V8" s="23"/>
       <c r="X8" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Y8" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Z8" s="21"/>
       <c r="AA8" s="23"/>
@@ -1713,12 +1809,18 @@
       <c r="AH8" s="23"/>
       <c r="AI8" s="21"/>
       <c r="AJ8" s="23"/>
-    </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A9" s="47" t="s">
+      <c r="AL8" s="21"/>
+      <c r="AM8" s="23"/>
+      <c r="AN8" s="21"/>
+      <c r="AO8" s="23"/>
+      <c r="AP8" s="21"/>
+      <c r="AQ8" s="23"/>
+    </row>
+    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A9" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="47"/>
+      <c r="B9" s="48"/>
       <c r="C9" s="2"/>
       <c r="D9" s="1" t="s">
         <v>46</v>
@@ -1744,20 +1846,20 @@
       <c r="O9" s="3"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R9" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="S9" s="21"/>
       <c r="T9" s="23"/>
       <c r="U9" s="21"/>
       <c r="V9" s="23"/>
       <c r="X9" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Y9" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Z9" s="21"/>
       <c r="AA9" s="23"/>
@@ -1769,12 +1871,18 @@
       <c r="AH9" s="23"/>
       <c r="AI9" s="21"/>
       <c r="AJ9" s="23"/>
-    </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A10" s="47" t="s">
+      <c r="AL9" s="21"/>
+      <c r="AM9" s="23"/>
+      <c r="AN9" s="21"/>
+      <c r="AO9" s="23"/>
+      <c r="AP9" s="21"/>
+      <c r="AQ9" s="23"/>
+    </row>
+    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A10" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="47"/>
+      <c r="B10" s="48"/>
       <c r="C10" s="2"/>
       <c r="D10" s="1" t="s">
         <v>46</v>
@@ -1798,24 +1906,24 @@
       <c r="M10" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="N10" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="O10" s="3"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="3">
+        <v>3.11</v>
+      </c>
       <c r="P10" s="4"/>
       <c r="Q10" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R10" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="S10" s="21"/>
       <c r="T10" s="23"/>
       <c r="U10" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="V10" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="X10" s="21"/>
       <c r="Y10" s="23"/>
@@ -1829,12 +1937,18 @@
       <c r="AH10" s="23"/>
       <c r="AI10" s="21"/>
       <c r="AJ10" s="23"/>
-    </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A11" s="47" t="s">
+      <c r="AL10" s="21"/>
+      <c r="AM10" s="23"/>
+      <c r="AN10" s="21"/>
+      <c r="AO10" s="23"/>
+      <c r="AP10" s="21"/>
+      <c r="AQ10" s="23"/>
+    </row>
+    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A11" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="47"/>
+      <c r="B11" s="48"/>
       <c r="C11" s="2"/>
       <c r="D11" s="1" t="s">
         <v>46</v>
@@ -1842,10 +1956,10 @@
       <c r="E11" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G11" s="3"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="3" t="s">
+        <v>124</v>
+      </c>
       <c r="H11" s="1" t="s">
         <v>46</v>
       </c>
@@ -1864,63 +1978,71 @@
       </c>
       <c r="N11" s="2"/>
       <c r="O11" s="3" t="s">
-        <v>92</v>
+        <v>127</v>
       </c>
       <c r="P11" s="4"/>
       <c r="Q11" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="R11" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="S11" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="T11" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="U11" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="R11" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="S11" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="T11" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="U11" s="21" t="s">
-        <v>111</v>
-      </c>
       <c r="V11" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X11" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Y11" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Z11" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AA11" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AB11" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AC11" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AE11" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AF11" s="23" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="AG11" s="21"/>
       <c r="AH11" s="23"/>
       <c r="AI11" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="AJ11" s="23"/>
-    </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A12" s="47" t="s">
+        <v>113</v>
+      </c>
+      <c r="AJ11" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="AL11" s="21"/>
+      <c r="AM11" s="23"/>
+      <c r="AN11" s="21"/>
+      <c r="AO11" s="23"/>
+      <c r="AP11" s="21"/>
+      <c r="AQ11" s="23"/>
+    </row>
+    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A12" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="47"/>
+      <c r="B12" s="48"/>
       <c r="C12" s="2"/>
       <c r="D12" s="1" t="s">
         <v>46</v>
@@ -1946,38 +2068,38 @@
         <v>46</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="N12" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="O12" s="3"/>
+        <v>92</v>
+      </c>
+      <c r="N12" s="2"/>
+      <c r="O12" s="3">
+        <v>3.8</v>
+      </c>
       <c r="P12" s="4"/>
       <c r="Q12" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="R12" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="S12" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="T12" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="U12" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="R12" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="S12" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="T12" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="U12" s="21" t="s">
-        <v>111</v>
-      </c>
       <c r="V12" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="X12" s="21"/>
       <c r="Y12" s="23"/>
       <c r="Z12" s="21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AA12" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AB12" s="21"/>
       <c r="AC12" s="23"/>
@@ -1987,12 +2109,18 @@
       <c r="AH12" s="23"/>
       <c r="AI12" s="21"/>
       <c r="AJ12" s="23"/>
-    </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A13" s="47" t="s">
+      <c r="AL12" s="21"/>
+      <c r="AM12" s="23"/>
+      <c r="AN12" s="21"/>
+      <c r="AO12" s="23"/>
+      <c r="AP12" s="21"/>
+      <c r="AQ12" s="23"/>
+    </row>
+    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A13" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="47"/>
+      <c r="B13" s="48"/>
       <c r="C13" s="2"/>
       <c r="D13" s="1" t="s">
         <v>46</v>
@@ -2000,25 +2128,25 @@
       <c r="E13" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G13" s="3"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="3">
+        <v>1.8</v>
+      </c>
       <c r="H13" s="1" t="s">
         <v>46</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="J13" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="K13" s="3"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="3">
+        <v>2.2999999999999998</v>
+      </c>
       <c r="L13" s="1" t="s">
         <v>46</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N13" s="2" t="s">
         <v>46</v>
@@ -2026,26 +2154,26 @@
       <c r="O13" s="3"/>
       <c r="P13" s="4"/>
       <c r="Q13" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R13" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="S13" s="21"/>
       <c r="T13" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="U13" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="V13" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="X13" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Y13" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Z13" s="21"/>
       <c r="AA13" s="23"/>
@@ -2057,12 +2185,18 @@
       <c r="AH13" s="23"/>
       <c r="AI13" s="21"/>
       <c r="AJ13" s="23"/>
-    </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A14" s="47" t="s">
+      <c r="AL13" s="21"/>
+      <c r="AM13" s="23"/>
+      <c r="AN13" s="21"/>
+      <c r="AO13" s="23"/>
+      <c r="AP13" s="21"/>
+      <c r="AQ13" s="23"/>
+    </row>
+    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A14" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="47"/>
+      <c r="B14" s="48"/>
       <c r="C14" s="2"/>
       <c r="D14" s="1" t="s">
         <v>46</v>
@@ -2070,10 +2204,10 @@
       <c r="E14" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="3">
-        <v>1.1000000000000001</v>
-      </c>
+      <c r="F14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" s="3"/>
       <c r="H14" s="1" t="s">
         <v>49</v>
       </c>
@@ -2088,128 +2222,148 @@
       <c r="O14" s="3"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R14" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="S14" s="21"/>
       <c r="T14" s="23"/>
       <c r="U14" s="21"/>
       <c r="V14" s="23"/>
       <c r="X14" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Y14" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Z14" s="21"/>
       <c r="AA14" s="23"/>
       <c r="AB14" s="21"/>
       <c r="AC14" s="23"/>
       <c r="AE14" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AF14" s="23" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="AG14" s="21"/>
       <c r="AH14" s="23"/>
       <c r="AI14" s="21"/>
       <c r="AJ14" s="23"/>
-    </row>
-    <row r="15" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="47" t="s">
+      <c r="AL14" s="21"/>
+      <c r="AM14" s="23"/>
+      <c r="AN14" s="21"/>
+      <c r="AO14" s="23"/>
+      <c r="AP14" s="21"/>
+      <c r="AQ14" s="23"/>
+    </row>
+    <row r="15" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="47"/>
+      <c r="B15" s="48"/>
       <c r="C15" s="2"/>
       <c r="D15" s="1" t="s">
         <v>46</v>
       </c>
       <c r="E15" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" s="3"/>
+      <c r="H15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I15" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="F15" s="2"/>
-      <c r="G15" s="3">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I15" s="26" t="s">
+      <c r="J15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K15" s="3"/>
+      <c r="L15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M15" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="J15" s="2"/>
-      <c r="K15" s="3">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="M15" s="26" t="s">
-        <v>118</v>
-      </c>
-      <c r="N15" s="2"/>
-      <c r="O15" s="3">
-        <v>4.0999999999999996</v>
+      <c r="N15" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="P15" s="4"/>
       <c r="Q15" s="27" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="R15" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="S15" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="S15" s="27" t="s">
-        <v>108</v>
-      </c>
       <c r="T15" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="U15" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="U15" s="27" t="s">
-        <v>108</v>
-      </c>
       <c r="V15" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="X15" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="X15" s="27" t="s">
-        <v>108</v>
-      </c>
       <c r="Y15" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="Z15" s="37" t="s">
         <v>107</v>
       </c>
-      <c r="Z15" s="37" t="s">
-        <v>108</v>
-      </c>
       <c r="AA15" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="AB15" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="AB15" s="27" t="s">
-        <v>108</v>
-      </c>
       <c r="AC15" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="AE15" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="AE15" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="AF15" s="28"/>
+      <c r="AF15" s="28" t="s">
+        <v>46</v>
+      </c>
       <c r="AG15" s="37" t="s">
-        <v>108</v>
-      </c>
-      <c r="AH15" s="28"/>
+        <v>107</v>
+      </c>
+      <c r="AH15" s="28" t="s">
+        <v>46</v>
+      </c>
       <c r="AI15" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="AJ15" s="28"/>
-    </row>
-    <row r="16" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="47" t="s">
+        <v>107</v>
+      </c>
+      <c r="AJ15" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="AL15" s="27"/>
+      <c r="AM15" s="28"/>
+      <c r="AN15" s="37"/>
+      <c r="AO15" s="28"/>
+      <c r="AP15" s="27"/>
+      <c r="AQ15" s="28"/>
+    </row>
+    <row r="16" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="47"/>
-      <c r="C16" s="47"/>
+      <c r="B16" s="48"/>
+      <c r="C16" s="48"/>
       <c r="D16" s="14"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
@@ -2241,12 +2395,18 @@
       <c r="AH16" s="31"/>
       <c r="AI16" s="32"/>
       <c r="AJ16" s="31"/>
-    </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A17" s="55" t="s">
+      <c r="AL16" s="32"/>
+      <c r="AM16" s="31"/>
+      <c r="AN16" s="32"/>
+      <c r="AO16" s="31"/>
+      <c r="AP16" s="32"/>
+      <c r="AQ16" s="31"/>
+    </row>
+    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A17" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="55"/>
+      <c r="B17" s="56"/>
       <c r="C17" s="2"/>
       <c r="D17" s="1" t="s">
         <v>46</v>
@@ -2272,10 +2432,10 @@
       <c r="O17" s="3"/>
       <c r="P17" s="4"/>
       <c r="Q17" s="29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R17" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="S17" s="29"/>
       <c r="T17" s="30"/>
@@ -2293,10 +2453,16 @@
       <c r="AH17" s="30"/>
       <c r="AI17" s="29"/>
       <c r="AJ17" s="30"/>
-    </row>
-    <row r="18" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="55"/>
-      <c r="B18" s="55"/>
+      <c r="AL17" s="29"/>
+      <c r="AM17" s="30"/>
+      <c r="AN17" s="29"/>
+      <c r="AO17" s="30"/>
+      <c r="AP17" s="29"/>
+      <c r="AQ17" s="30"/>
+    </row>
+    <row r="18" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="56"/>
+      <c r="B18" s="56"/>
       <c r="C18" s="2"/>
       <c r="D18" s="1" t="s">
         <v>46</v>
@@ -2322,10 +2488,10 @@
       <c r="O18" s="3"/>
       <c r="P18" s="4"/>
       <c r="Q18" s="27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R18" s="28" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="S18" s="27"/>
       <c r="T18" s="28"/>
@@ -2343,12 +2509,18 @@
       <c r="AH18" s="28"/>
       <c r="AI18" s="27"/>
       <c r="AJ18" s="28"/>
-    </row>
-    <row r="19" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="48" t="s">
+      <c r="AL18" s="27"/>
+      <c r="AM18" s="28"/>
+      <c r="AN18" s="27"/>
+      <c r="AO18" s="28"/>
+      <c r="AP18" s="27"/>
+      <c r="AQ18" s="28"/>
+    </row>
+    <row r="19" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="48"/>
+      <c r="B19" s="49"/>
       <c r="C19" s="2" t="s">
         <v>50</v>
       </c>
@@ -2387,12 +2559,18 @@
       <c r="AH19" s="31"/>
       <c r="AI19" s="32"/>
       <c r="AJ19" s="31"/>
-    </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A20" s="48" t="s">
+      <c r="AL19" s="32"/>
+      <c r="AM19" s="31"/>
+      <c r="AN19" s="32"/>
+      <c r="AO19" s="31"/>
+      <c r="AP19" s="32"/>
+      <c r="AQ19" s="31"/>
+    </row>
+    <row r="20" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A20" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="48"/>
+      <c r="B20" s="49"/>
       <c r="C20" s="2"/>
       <c r="D20" s="1" t="s">
         <v>46</v>
@@ -2418,7 +2596,7 @@
         <v>46</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N20" s="2" t="s">
         <v>46</v>
@@ -2426,20 +2604,20 @@
       <c r="O20" s="3"/>
       <c r="P20" s="4"/>
       <c r="Q20" s="29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R20" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="S20" s="29"/>
       <c r="T20" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="U20" s="29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="V20" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="X20" s="29"/>
       <c r="Y20" s="30"/>
@@ -2453,12 +2631,18 @@
       <c r="AH20" s="30"/>
       <c r="AI20" s="29"/>
       <c r="AJ20" s="30"/>
-    </row>
-    <row r="21" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="48" t="s">
+      <c r="AL20" s="29"/>
+      <c r="AM20" s="30"/>
+      <c r="AN20" s="29"/>
+      <c r="AO20" s="30"/>
+      <c r="AP20" s="29"/>
+      <c r="AQ20" s="30"/>
+    </row>
+    <row r="21" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="48"/>
+      <c r="B21" s="49"/>
       <c r="C21" s="2"/>
       <c r="D21" s="1" t="s">
         <v>46</v>
@@ -2484,7 +2668,7 @@
         <v>46</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N21" s="2" t="s">
         <v>46</v>
@@ -2492,20 +2676,20 @@
       <c r="O21" s="3"/>
       <c r="P21" s="4"/>
       <c r="Q21" s="27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R21" s="28" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="S21" s="27"/>
       <c r="T21" s="28" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="U21" s="27" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="V21" s="28" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="X21" s="27"/>
       <c r="Y21" s="28"/>
@@ -2519,13 +2703,19 @@
       <c r="AH21" s="28"/>
       <c r="AI21" s="27"/>
       <c r="AJ21" s="28"/>
-    </row>
-    <row r="22" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="47" t="s">
+      <c r="AL21" s="27"/>
+      <c r="AM21" s="28"/>
+      <c r="AN21" s="27"/>
+      <c r="AO21" s="28"/>
+      <c r="AP21" s="27"/>
+      <c r="AQ21" s="28"/>
+    </row>
+    <row r="22" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="47"/>
-      <c r="C22" s="47"/>
+      <c r="B22" s="48"/>
+      <c r="C22" s="48"/>
       <c r="D22" s="14"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
@@ -2557,12 +2747,18 @@
       <c r="AH22" s="31"/>
       <c r="AI22" s="32"/>
       <c r="AJ22" s="31"/>
-    </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A23" s="48" t="s">
+      <c r="AL22" s="32"/>
+      <c r="AM22" s="31"/>
+      <c r="AN22" s="32"/>
+      <c r="AO22" s="31"/>
+      <c r="AP22" s="32"/>
+      <c r="AQ22" s="31"/>
+    </row>
+    <row r="23" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A23" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="48"/>
+      <c r="B23" s="49"/>
       <c r="C23" s="2"/>
       <c r="D23" s="1" t="s">
         <v>46</v>
@@ -2592,47 +2788,53 @@
       <c r="O23" s="3"/>
       <c r="P23" s="4"/>
       <c r="Q23" s="29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R23" s="30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="S23" s="29"/>
       <c r="T23" s="30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="U23" s="29"/>
       <c r="V23" s="30"/>
       <c r="X23" s="29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Y23" s="30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Z23" s="29" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AA23" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AB23" s="29"/>
       <c r="AC23" s="30"/>
       <c r="AE23" s="29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AF23" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AG23" s="29"/>
       <c r="AH23" s="30"/>
       <c r="AI23" s="29"/>
       <c r="AJ23" s="30"/>
-    </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A24" s="48" t="s">
+      <c r="AL23" s="29"/>
+      <c r="AM23" s="30"/>
+      <c r="AN23" s="29"/>
+      <c r="AO23" s="30"/>
+      <c r="AP23" s="29"/>
+      <c r="AQ23" s="30"/>
+    </row>
+    <row r="24" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A24" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="48"/>
+      <c r="B24" s="49"/>
       <c r="C24" s="2"/>
       <c r="D24" s="1" t="s">
         <v>46</v>
@@ -2640,10 +2842,10 @@
       <c r="E24" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F24" s="2"/>
-      <c r="G24" s="19">
-        <v>1.1000000000000001</v>
-      </c>
+      <c r="F24" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G24" s="19"/>
       <c r="H24" s="1" t="s">
         <v>46</v>
       </c>
@@ -2662,51 +2864,57 @@
       <c r="O24" s="19"/>
       <c r="P24" s="4"/>
       <c r="Q24" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R24" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="S24" s="21"/>
       <c r="T24" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="U24" s="21"/>
       <c r="V24" s="23"/>
       <c r="X24" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Y24" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Z24" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AA24" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AB24" s="21"/>
       <c r="AC24" s="23"/>
       <c r="AE24" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AF24" s="23" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AG24" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AH24" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AI24" s="21"/>
       <c r="AJ24" s="23"/>
-    </row>
-    <row r="25" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="48" t="s">
+      <c r="AL24" s="21"/>
+      <c r="AM24" s="23"/>
+      <c r="AN24" s="21"/>
+      <c r="AO24" s="23"/>
+      <c r="AP24" s="21"/>
+      <c r="AQ24" s="23"/>
+    </row>
+    <row r="25" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="48"/>
+      <c r="B25" s="49"/>
       <c r="C25" s="2"/>
       <c r="D25" s="1" t="s">
         <v>46</v>
@@ -2714,10 +2922,10 @@
       <c r="E25" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F25" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G25" s="3"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="3">
+        <v>1.7</v>
+      </c>
       <c r="H25" s="1" t="s">
         <v>46</v>
       </c>
@@ -2732,60 +2940,68 @@
         <v>46</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N25" s="2"/>
-      <c r="O25" s="3">
-        <v>3.4</v>
+      <c r="O25" s="3" t="s">
+        <v>128</v>
       </c>
       <c r="P25" s="4"/>
       <c r="Q25" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="R25" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="S25" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="T25" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="U25" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="R25" s="28" t="s">
-        <v>109</v>
-      </c>
-      <c r="S25" s="27" t="s">
-        <v>106</v>
-      </c>
-      <c r="T25" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="U25" s="27" t="s">
-        <v>111</v>
-      </c>
       <c r="V25" s="28" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X25" s="27"/>
       <c r="Y25" s="28"/>
       <c r="Z25" s="27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AA25" s="28" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AB25" s="27" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AC25" s="28" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AE25" s="27"/>
       <c r="AF25" s="28"/>
       <c r="AG25" s="27"/>
       <c r="AH25" s="28"/>
       <c r="AI25" s="27" t="s">
-        <v>114</v>
-      </c>
-      <c r="AJ25" s="28"/>
-    </row>
-    <row r="26" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="47" t="s">
+        <v>113</v>
+      </c>
+      <c r="AJ25" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="AL25" s="27"/>
+      <c r="AM25" s="28"/>
+      <c r="AN25" s="27"/>
+      <c r="AO25" s="28"/>
+      <c r="AP25" s="27"/>
+      <c r="AQ25" s="28"/>
+    </row>
+    <row r="26" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="47"/>
-      <c r="C26" s="47"/>
+      <c r="B26" s="48"/>
+      <c r="C26" s="48"/>
       <c r="D26" s="14"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
@@ -2817,12 +3033,18 @@
       <c r="AH26" s="31"/>
       <c r="AI26" s="32"/>
       <c r="AJ26" s="31"/>
-    </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A27" s="48" t="s">
+      <c r="AL26" s="32"/>
+      <c r="AM26" s="31"/>
+      <c r="AN26" s="32"/>
+      <c r="AO26" s="31"/>
+      <c r="AP26" s="32"/>
+      <c r="AQ26" s="31"/>
+    </row>
+    <row r="27" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A27" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="48"/>
+      <c r="B27" s="49"/>
       <c r="C27" s="2"/>
       <c r="D27" s="1" t="s">
         <v>49</v>
@@ -2836,65 +3058,73 @@
       <c r="I27" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="J27" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="K27" s="3"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="3">
+        <v>2.5</v>
+      </c>
       <c r="L27" s="1" t="s">
         <v>46</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N27" s="2"/>
-      <c r="O27" s="3">
-        <v>3.5</v>
+      <c r="O27" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="P27" s="4"/>
       <c r="Q27" s="29"/>
       <c r="R27" s="30"/>
       <c r="S27" s="29"/>
       <c r="T27" s="30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="U27" s="29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="V27" s="30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X27" s="29"/>
       <c r="Y27" s="30"/>
       <c r="Z27" s="29" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AA27" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="AB27" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="AB27" s="29" t="s">
-        <v>108</v>
-      </c>
       <c r="AC27" s="30" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AE27" s="29"/>
       <c r="AF27" s="30"/>
       <c r="AG27" s="29" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AH27" s="30" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="AI27" s="29" t="s">
-        <v>114</v>
-      </c>
-      <c r="AJ27" s="30"/>
-    </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A28" s="48" t="s">
+        <v>113</v>
+      </c>
+      <c r="AJ27" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="AL27" s="29"/>
+      <c r="AM27" s="30"/>
+      <c r="AN27" s="29"/>
+      <c r="AO27" s="30"/>
+      <c r="AP27" s="29"/>
+      <c r="AQ27" s="30"/>
+    </row>
+    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A28" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="48"/>
+      <c r="B28" s="49"/>
       <c r="C28" s="2"/>
       <c r="D28" s="1" t="s">
         <v>49</v>
@@ -2918,61 +3148,69 @@
         <v>46</v>
       </c>
       <c r="M28" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="N28" s="2"/>
-      <c r="O28" s="3">
-        <v>1.8</v>
+      <c r="O28" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="P28" s="4"/>
       <c r="Q28" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R28" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="S28" s="21"/>
       <c r="T28" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="U28" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="V28" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X28" s="21"/>
       <c r="Y28" s="23"/>
       <c r="Z28" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AA28" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="AB28" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="AB28" s="21" t="s">
-        <v>108</v>
-      </c>
       <c r="AC28" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AE28" s="21"/>
       <c r="AF28" s="23"/>
       <c r="AG28" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AH28" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AI28" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="AJ28" s="23"/>
-    </row>
-    <row r="29" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="48" t="s">
+        <v>113</v>
+      </c>
+      <c r="AJ28" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="AL28" s="21"/>
+      <c r="AM28" s="23"/>
+      <c r="AN28" s="21"/>
+      <c r="AO28" s="23"/>
+      <c r="AP28" s="21"/>
+      <c r="AQ28" s="23"/>
+    </row>
+    <row r="29" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="48"/>
+      <c r="B29" s="49"/>
       <c r="C29" s="2"/>
       <c r="D29" s="1" t="s">
         <v>46</v>
@@ -2980,72 +3218,80 @@
       <c r="E29" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F29" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G29" s="3"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="3">
+        <v>1.3</v>
+      </c>
       <c r="H29" s="1" t="s">
         <v>46</v>
       </c>
       <c r="I29" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="J29" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="K29" s="3"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="3">
+        <v>2.1</v>
+      </c>
       <c r="L29" s="1" t="s">
         <v>46</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N29" s="2"/>
-      <c r="O29" s="3">
-        <v>3.6</v>
+      <c r="O29" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="P29" s="4"/>
       <c r="Q29" s="27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R29" s="28" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="S29" s="27"/>
       <c r="T29" s="28" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="U29" s="27" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="V29" s="28" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X29" s="27"/>
       <c r="Y29" s="28"/>
       <c r="Z29" s="27"/>
       <c r="AA29" s="28"/>
       <c r="AB29" s="27" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AC29" s="28" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AE29" s="27"/>
       <c r="AF29" s="28"/>
       <c r="AG29" s="27"/>
       <c r="AH29" s="28"/>
       <c r="AI29" s="27" t="s">
-        <v>114</v>
-      </c>
-      <c r="AJ29" s="28"/>
-    </row>
-    <row r="30" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="47" t="s">
+        <v>113</v>
+      </c>
+      <c r="AJ29" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="AL29" s="27"/>
+      <c r="AM29" s="28"/>
+      <c r="AN29" s="27"/>
+      <c r="AO29" s="28"/>
+      <c r="AP29" s="27"/>
+      <c r="AQ29" s="28"/>
+    </row>
+    <row r="30" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="47"/>
-      <c r="C30" s="47"/>
+      <c r="B30" s="48"/>
+      <c r="C30" s="48"/>
       <c r="D30" s="14"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
@@ -3078,12 +3324,18 @@
       <c r="AH30" s="31"/>
       <c r="AI30" s="32"/>
       <c r="AJ30" s="31"/>
-    </row>
-    <row r="31" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="48" t="s">
+      <c r="AL30" s="32"/>
+      <c r="AM30" s="31"/>
+      <c r="AN30" s="32"/>
+      <c r="AO30" s="31"/>
+      <c r="AP30" s="32"/>
+      <c r="AQ30" s="31"/>
+    </row>
+    <row r="31" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="48"/>
+      <c r="B31" s="49"/>
       <c r="C31" s="2"/>
       <c r="D31" s="1" t="s">
         <v>46</v>
@@ -3091,10 +3343,10 @@
       <c r="E31" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F31" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G31" s="3"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="38">
+        <v>1.1000000000000001</v>
+      </c>
       <c r="H31" s="1" t="s">
         <v>49</v>
       </c>
@@ -3126,12 +3378,18 @@
       <c r="AH31" s="36"/>
       <c r="AI31" s="35"/>
       <c r="AJ31" s="36"/>
-    </row>
-    <row r="32" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="48" t="s">
+      <c r="AL31" s="35"/>
+      <c r="AM31" s="36"/>
+      <c r="AN31" s="35"/>
+      <c r="AO31" s="36"/>
+      <c r="AP31" s="35"/>
+      <c r="AQ31" s="36"/>
+    </row>
+    <row r="32" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="B32" s="48"/>
+      <c r="B32" s="49"/>
       <c r="C32" s="2" t="s">
         <v>50</v>
       </c>
@@ -3170,12 +3428,18 @@
       <c r="AH32" s="31"/>
       <c r="AI32" s="32"/>
       <c r="AJ32" s="31"/>
-    </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A33" s="48" t="s">
+      <c r="AL32" s="32"/>
+      <c r="AM32" s="31"/>
+      <c r="AN32" s="32"/>
+      <c r="AO32" s="31"/>
+      <c r="AP32" s="32"/>
+      <c r="AQ32" s="31"/>
+    </row>
+    <row r="33" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A33" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="B33" s="48"/>
+      <c r="B33" s="49"/>
       <c r="C33" s="2"/>
       <c r="D33" s="1" t="s">
         <v>46</v>
@@ -3201,20 +3465,20 @@
       <c r="O33" s="3"/>
       <c r="P33" s="4"/>
       <c r="Q33" s="29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R33" s="30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="S33" s="29"/>
       <c r="T33" s="30"/>
       <c r="U33" s="29"/>
       <c r="V33" s="30"/>
       <c r="X33" s="29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Y33" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Z33" s="29"/>
       <c r="AA33" s="30"/>
@@ -3226,12 +3490,18 @@
       <c r="AH33" s="30"/>
       <c r="AI33" s="29"/>
       <c r="AJ33" s="30"/>
-    </row>
-    <row r="34" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="48" t="s">
+      <c r="AL33" s="29"/>
+      <c r="AM33" s="30"/>
+      <c r="AN33" s="29"/>
+      <c r="AO33" s="30"/>
+      <c r="AP33" s="29"/>
+      <c r="AQ33" s="30"/>
+    </row>
+    <row r="34" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="48"/>
+      <c r="B34" s="49"/>
       <c r="C34" s="2"/>
       <c r="D34" s="1" t="s">
         <v>46</v>
@@ -3239,25 +3509,25 @@
       <c r="E34" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F34" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G34" s="3"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="3" t="s">
+        <v>123</v>
+      </c>
       <c r="H34" s="1" t="s">
         <v>46</v>
       </c>
       <c r="I34" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="J34" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="K34" s="3"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="3" t="s">
+        <v>125</v>
+      </c>
       <c r="L34" s="1" t="s">
         <v>46</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N34" s="2" t="s">
         <v>46</v>
@@ -3265,28 +3535,28 @@
       <c r="O34" s="3"/>
       <c r="P34" s="4"/>
       <c r="Q34" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="R34" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="S34" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="T34" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="U34" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="R34" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="S34" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="T34" s="28" t="s">
-        <v>109</v>
-      </c>
-      <c r="U34" s="27" t="s">
-        <v>111</v>
-      </c>
       <c r="V34" s="28" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="X34" s="27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Y34" s="28" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Z34" s="27"/>
       <c r="AA34" s="28"/>
@@ -3298,13 +3568,19 @@
       <c r="AH34" s="28"/>
       <c r="AI34" s="27"/>
       <c r="AJ34" s="28"/>
-    </row>
-    <row r="35" spans="1:36" s="11" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="47" t="s">
+      <c r="AL34" s="27"/>
+      <c r="AM34" s="28"/>
+      <c r="AN34" s="27"/>
+      <c r="AO34" s="28"/>
+      <c r="AP34" s="27"/>
+      <c r="AQ34" s="28"/>
+    </row>
+    <row r="35" spans="1:43" s="11" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="B35" s="47"/>
-      <c r="C35" s="47"/>
+      <c r="B35" s="48"/>
+      <c r="C35" s="48"/>
       <c r="D35" s="14"/>
       <c r="E35" s="9"/>
       <c r="F35" s="9"/>
@@ -3336,12 +3612,18 @@
       <c r="AH35" s="33"/>
       <c r="AI35" s="32"/>
       <c r="AJ35" s="33"/>
-    </row>
-    <row r="36" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A36" s="48" t="s">
+      <c r="AL35" s="32"/>
+      <c r="AM35" s="33"/>
+      <c r="AN35" s="34"/>
+      <c r="AO35" s="33"/>
+      <c r="AP35" s="32"/>
+      <c r="AQ35" s="33"/>
+    </row>
+    <row r="36" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A36" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="B36" s="48"/>
+      <c r="B36" s="49"/>
       <c r="C36" s="2"/>
       <c r="D36" s="1" t="s">
         <v>46</v>
@@ -3367,10 +3649,10 @@
       <c r="O36" s="3"/>
       <c r="P36" s="4"/>
       <c r="Q36" s="29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R36" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="S36" s="29"/>
       <c r="T36" s="30"/>
@@ -3388,12 +3670,18 @@
       <c r="AH36" s="30"/>
       <c r="AI36" s="29"/>
       <c r="AJ36" s="30"/>
-    </row>
-    <row r="37" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A37" s="48" t="s">
+      <c r="AL36" s="29"/>
+      <c r="AM36" s="30"/>
+      <c r="AN36" s="29"/>
+      <c r="AO36" s="30"/>
+      <c r="AP36" s="29"/>
+      <c r="AQ36" s="30"/>
+    </row>
+    <row r="37" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A37" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="B37" s="48"/>
+      <c r="B37" s="49"/>
       <c r="C37" s="2"/>
       <c r="D37" s="1" t="s">
         <v>46</v>
@@ -3417,10 +3705,10 @@
       <c r="O37" s="3"/>
       <c r="P37" s="4"/>
       <c r="Q37" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R37" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="S37" s="21"/>
       <c r="T37" s="23"/>
@@ -3438,12 +3726,18 @@
       <c r="AH37" s="23"/>
       <c r="AI37" s="21"/>
       <c r="AJ37" s="23"/>
-    </row>
-    <row r="38" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A38" s="48" t="s">
+      <c r="AL37" s="21"/>
+      <c r="AM37" s="23"/>
+      <c r="AN37" s="21"/>
+      <c r="AO37" s="23"/>
+      <c r="AP37" s="21"/>
+      <c r="AQ37" s="23"/>
+    </row>
+    <row r="38" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A38" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="B38" s="48"/>
+      <c r="B38" s="49"/>
       <c r="C38" s="2"/>
       <c r="D38" s="1" t="s">
         <v>46</v>
@@ -3451,10 +3745,10 @@
       <c r="E38" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F38" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G38" s="3"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="3">
+        <v>1.9</v>
+      </c>
       <c r="H38" s="1" t="s">
         <v>49</v>
       </c>
@@ -3469,20 +3763,20 @@
       <c r="O38" s="3"/>
       <c r="P38" s="4"/>
       <c r="Q38" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R38" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="S38" s="21"/>
       <c r="T38" s="23"/>
       <c r="U38" s="21"/>
       <c r="V38" s="23"/>
       <c r="X38" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Y38" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Z38" s="21"/>
       <c r="AA38" s="23"/>
@@ -3494,12 +3788,18 @@
       <c r="AH38" s="23"/>
       <c r="AI38" s="21"/>
       <c r="AJ38" s="23"/>
-    </row>
-    <row r="39" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="48" t="s">
+      <c r="AL38" s="21"/>
+      <c r="AM38" s="23"/>
+      <c r="AN38" s="21"/>
+      <c r="AO38" s="23"/>
+      <c r="AP38" s="21"/>
+      <c r="AQ38" s="23"/>
+    </row>
+    <row r="39" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="B39" s="48"/>
+      <c r="B39" s="49"/>
       <c r="C39" s="2"/>
       <c r="D39" s="1" t="s">
         <v>46</v>
@@ -3521,56 +3821,64 @@
         <v>46</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N39" s="2"/>
       <c r="O39" s="3">
-        <v>3.1</v>
+        <v>3.12</v>
       </c>
       <c r="P39" s="4"/>
       <c r="Q39" s="27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R39" s="28" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="S39" s="27"/>
       <c r="T39" s="28"/>
       <c r="U39" s="27" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="V39" s="28" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X39" s="27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Y39" s="28" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Z39" s="27"/>
       <c r="AA39" s="28"/>
       <c r="AB39" s="27" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AC39" s="28" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AE39" s="27"/>
       <c r="AF39" s="28"/>
       <c r="AG39" s="27"/>
       <c r="AH39" s="28"/>
       <c r="AI39" s="27" t="s">
-        <v>114</v>
-      </c>
-      <c r="AJ39" s="28"/>
-    </row>
-    <row r="40" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="47" t="s">
+        <v>113</v>
+      </c>
+      <c r="AJ39" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="AL39" s="27"/>
+      <c r="AM39" s="28"/>
+      <c r="AN39" s="27"/>
+      <c r="AO39" s="28"/>
+      <c r="AP39" s="27"/>
+      <c r="AQ39" s="28"/>
+    </row>
+    <row r="40" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="B40" s="47"/>
-      <c r="C40" s="47"/>
+      <c r="B40" s="48"/>
+      <c r="C40" s="48"/>
       <c r="D40" s="14"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
@@ -3602,12 +3910,18 @@
       <c r="AH40" s="31"/>
       <c r="AI40" s="32"/>
       <c r="AJ40" s="31"/>
-    </row>
-    <row r="41" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="48" t="s">
+      <c r="AL40" s="32"/>
+      <c r="AM40" s="31"/>
+      <c r="AN40" s="32"/>
+      <c r="AO40" s="31"/>
+      <c r="AP40" s="32"/>
+      <c r="AQ40" s="31"/>
+    </row>
+    <row r="41" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="B41" s="48"/>
+      <c r="B41" s="49"/>
       <c r="C41" s="2"/>
       <c r="D41" s="1" t="s">
         <v>46</v>
@@ -3633,10 +3947,10 @@
       <c r="O41" s="3"/>
       <c r="P41" s="4"/>
       <c r="Q41" s="35" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R41" s="36" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="S41" s="35"/>
       <c r="T41" s="36"/>
@@ -3654,12 +3968,18 @@
       <c r="AH41" s="36"/>
       <c r="AI41" s="35"/>
       <c r="AJ41" s="36"/>
-    </row>
-    <row r="42" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="48" t="s">
+      <c r="AL41" s="35"/>
+      <c r="AM41" s="36"/>
+      <c r="AN41" s="35"/>
+      <c r="AO41" s="36"/>
+      <c r="AP41" s="35"/>
+      <c r="AQ41" s="36"/>
+    </row>
+    <row r="42" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="48"/>
+      <c r="B42" s="49"/>
       <c r="C42" s="2" t="s">
         <v>50</v>
       </c>
@@ -3700,12 +4020,18 @@
       <c r="AH42" s="31"/>
       <c r="AI42" s="32"/>
       <c r="AJ42" s="31"/>
-    </row>
-    <row r="43" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A43" s="48" t="s">
+      <c r="AL42" s="32"/>
+      <c r="AM42" s="31"/>
+      <c r="AN42" s="32"/>
+      <c r="AO42" s="31"/>
+      <c r="AP42" s="32"/>
+      <c r="AQ42" s="31"/>
+    </row>
+    <row r="43" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A43" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="B43" s="48"/>
+      <c r="B43" s="49"/>
       <c r="C43" s="2"/>
       <c r="D43" s="1"/>
       <c r="E43" s="2" t="s">
@@ -3729,10 +4055,10 @@
       <c r="O43" s="3"/>
       <c r="P43" s="4"/>
       <c r="Q43" s="29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R43" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="S43" s="29"/>
       <c r="T43" s="30"/>
@@ -3750,12 +4076,18 @@
       <c r="AH43" s="30"/>
       <c r="AI43" s="29"/>
       <c r="AJ43" s="30"/>
-    </row>
-    <row r="44" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="48" t="s">
+      <c r="AL43" s="29"/>
+      <c r="AM43" s="30"/>
+      <c r="AN43" s="29"/>
+      <c r="AO43" s="30"/>
+      <c r="AP43" s="29"/>
+      <c r="AQ43" s="30"/>
+    </row>
+    <row r="44" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="B44" s="48"/>
+      <c r="B44" s="49"/>
       <c r="C44" s="2"/>
       <c r="D44" s="5" t="s">
         <v>46</v>
@@ -3781,10 +4113,10 @@
       <c r="O44" s="7"/>
       <c r="P44" s="4"/>
       <c r="Q44" s="22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R44" s="24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="S44" s="22"/>
       <c r="T44" s="24"/>
@@ -3802,36 +4134,29 @@
       <c r="AH44" s="24"/>
       <c r="AI44" s="22"/>
       <c r="AJ44" s="24"/>
-    </row>
-    <row r="45" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AL44" s="22"/>
+      <c r="AM44" s="24"/>
+      <c r="AN44" s="22"/>
+      <c r="AO44" s="24"/>
+      <c r="AP44" s="22"/>
+      <c r="AQ44" s="24"/>
+    </row>
+    <row r="45" spans="1:43" x14ac:dyDescent="0.25">
       <c r="D45" s="13"/>
       <c r="U45" s="4"/>
     </row>
-    <row r="46" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="AE46" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="47" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="AE47" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="48" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="AE48" t="s">
-        <v>123</v>
+    <row r="47" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AL47" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="48" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AL48" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="58">
-    <mergeCell ref="AE2:AJ2"/>
-    <mergeCell ref="AE3:AF3"/>
-    <mergeCell ref="AG3:AH3"/>
-    <mergeCell ref="AI3:AJ3"/>
-    <mergeCell ref="X2:AC2"/>
-    <mergeCell ref="X3:Y3"/>
-    <mergeCell ref="Z3:AA3"/>
-    <mergeCell ref="AB3:AC3"/>
+  <mergeCells count="62">
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A3:C3"/>
@@ -3865,8 +4190,6 @@
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A41:B41"/>
     <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A15:B15"/>
@@ -3875,13 +4198,27 @@
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="E2:O2"/>
+    <mergeCell ref="L3:O3"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="AL2:AQ2"/>
+    <mergeCell ref="AL3:AM3"/>
+    <mergeCell ref="AN3:AO3"/>
+    <mergeCell ref="AP3:AQ3"/>
     <mergeCell ref="Q2:V2"/>
     <mergeCell ref="Q3:R3"/>
     <mergeCell ref="S3:T3"/>
     <mergeCell ref="U3:V3"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="E2:O2"/>
-    <mergeCell ref="L3:O3"/>
+    <mergeCell ref="AE2:AJ2"/>
+    <mergeCell ref="AE3:AF3"/>
+    <mergeCell ref="AG3:AH3"/>
+    <mergeCell ref="AI3:AJ3"/>
+    <mergeCell ref="X2:AC2"/>
+    <mergeCell ref="X3:Y3"/>
+    <mergeCell ref="Z3:AA3"/>
+    <mergeCell ref="AB3:AC3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3900,7 +4237,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>